<commit_message>
update api & mobile testing
</commit_message>
<xml_diff>
--- a/Data Test/edit_profile.xlsx
+++ b/Data Test/edit_profile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. UNNES\6. Semester 6\2 - MSIB\CAPSTONE PROJECT\testing-lms\Data Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC97B4E0-A78A-449B-BC66-A82DE8F59769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15B89B2-67CA-4338-8ED7-58E3E3DA5817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="18000" windowHeight="9270" xr2:uid="{45076FA3-564A-4E50-94CC-5AE5A21FCC3F}"/>
+    <workbookView xWindow="4170" yWindow="1470" windowWidth="18000" windowHeight="9270" xr2:uid="{45076FA3-564A-4E50-94CC-5AE5A21FCC3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>email</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>archen1@gmail.com</t>
+  </si>
+  <si>
+    <t>Sa</t>
+  </si>
+  <si>
+    <t>sal@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -493,7 +499,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,10 +588,10 @@
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
update data test for web, mobile, and api
</commit_message>
<xml_diff>
--- a/Data Test/edit_profile.xlsx
+++ b/Data Test/edit_profile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. UNNES\6. Semester 6\2 - MSIB\CAPSTONE PROJECT\testing-lms\Data Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635B4146-BA6B-44BE-B489-601C47DC5306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848BC146-D570-476F-ABF5-457725886C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="1245" windowWidth="18000" windowHeight="9270" xr2:uid="{45076FA3-564A-4E50-94CC-5AE5A21FCC3F}"/>
+    <workbookView xWindow="2445" yWindow="2205" windowWidth="18000" windowHeight="9270" xr2:uid="{45076FA3-564A-4E50-94CC-5AE5A21FCC3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>arch-gmail</t>
-  </si>
-  <si>
     <t>tc-id</t>
   </si>
   <si>
@@ -74,19 +71,22 @@
     <t>no_telp</t>
   </si>
   <si>
-    <t>081234562377</t>
-  </si>
-  <si>
     <t>0812345</t>
   </si>
   <si>
-    <t>archen1@gmail.com</t>
-  </si>
-  <si>
-    <t>Joong</t>
-  </si>
-  <si>
     <t>joongs@gmail.com</t>
+  </si>
+  <si>
+    <t>joong</t>
+  </si>
+  <si>
+    <t>Joong A</t>
+  </si>
+  <si>
+    <t>08123456789</t>
+  </si>
+  <si>
+    <t>joong@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -496,7 +496,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C2:C5"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,87 +511,87 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>